<commit_message>
Last row Check redundancy state - lh coremp mirror stat, st SwitchInternalLink, get SwitchCoreUnit state New Criteria
</commit_message>
<xml_diff>
--- a/Criteria.xlsx
+++ b/Criteria.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="135" windowWidth="19980" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="168">
   <si>
     <t>Check active Alarms</t>
   </si>
@@ -84,21 +82,9 @@
     <t>Что ищет парсер</t>
   </si>
   <si>
-    <t>alt - команда</t>
-  </si>
-  <si>
-    <t>Total: * Alarms (* Critical, * Major)</t>
-  </si>
-  <si>
     <t>Исключения</t>
   </si>
   <si>
-    <t>lgesmr 7d - команда</t>
-  </si>
-  <si>
-    <t>lgd - команда</t>
-  </si>
-  <si>
     <t>Например:</t>
   </si>
   <si>
@@ -210,9 +196,6 @@
     <t>M3uAssociation=ps** в графе Op. State значение disabled ≥2шт.</t>
   </si>
   <si>
-    <t>M3uAssociation=rs** в графе Op. State значение disabled 1шт.</t>
-  </si>
-  <si>
     <t>std</t>
   </si>
   <si>
@@ -255,16 +238,10 @@
     <t>lhsh 00**00 readclock</t>
   </si>
   <si>
-    <t>при условии, что "Site availability:  AA of BB" (BB-AA)≥5</t>
-  </si>
-  <si>
     <t>powertest; STEP30; delivery для Spontaneous RestartType/Reason</t>
   </si>
   <si>
     <t>AA of BB unlocked cells are up (#.# %), где процентаж от 0 до 90</t>
-  </si>
-  <si>
-    <t>и (BB-AA)≥40</t>
   </si>
   <si>
     <r>
@@ -293,12 +270,6 @@
     </r>
   </si>
   <si>
-    <t>и (BB-AA)≥20</t>
-  </si>
-  <si>
-    <t>и (BB-AA)≥10</t>
-  </si>
-  <si>
     <t>* of * unlocked cells are up (**.* %)</t>
   </si>
   <si>
@@ -317,9 +288,6 @@
     <t>Какая-либо M3ua в графе Op. State значение disabled</t>
   </si>
   <si>
-    <t>при условии, что "Site availability:  AA of BB" (BB-AA)≤5</t>
-  </si>
-  <si>
     <t>Если CFRPHEU* (1-6) в статусе L*****</t>
   </si>
   <si>
@@ -525,13 +493,61 @@
   </si>
   <si>
     <t>stip</t>
+  </si>
+  <si>
+    <t>Alarms_and_events.xlsx</t>
+  </si>
+  <si>
+    <t>Total: * Alarms (* Critical, * Major, * Minor, * Warning)</t>
+  </si>
+  <si>
+    <t>Список исключений надо добавить отдельным списком, в</t>
+  </si>
+  <si>
+    <t>котором будут указаны аварии, которые не должны учитываться</t>
+  </si>
+  <si>
+    <t>при присвоении статуса в выгрузке.</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>lgesmr 7d</t>
+  </si>
+  <si>
+    <t>lgd</t>
+  </si>
+  <si>
+    <t>M3uAssociation=rs** в графе Op. State значение disabled ≥1шт.</t>
+  </si>
+  <si>
+    <t>и (BB-AA)≥40 pieces</t>
+  </si>
+  <si>
+    <t>и (BB-AA)≥20 pieces</t>
+  </si>
+  <si>
+    <t>и (BB-AA)≥10 pieces</t>
+  </si>
+  <si>
+    <t>при условии, что "Site availability:  AA of BB" (BB-AA)≤5 pieces</t>
+  </si>
+  <si>
+    <t>при условии, что "Site availability:  AA of BB" (BB-AA)≥5 pieces</t>
+  </si>
+  <si>
+    <t>если не [linkEstablished synced allocatedSp allocatedRh] для DC/CC</t>
+  </si>
+  <si>
+    <t>если не [linkEstablished allocatedSp allocatedRh] для PDR</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -586,6 +602,15 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="8">
@@ -759,18 +784,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -802,10 +823,12 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -818,9 +841,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Стандартная">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -858,7 +881,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Стандартная">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -892,6 +915,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -926,9 +950,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Стандартная">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1101,1058 +1126,1050 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C5" sqref="C5"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="8" width="60.7109375" style="6" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="8" width="60.7109375" style="4" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="15" customHeight="1">
-      <c r="A2" s="14" t="s">
+      <c r="C1" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>22</v>
+        <v>157</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" ht="15" customHeight="1">
-      <c r="A3" s="15"/>
+        <v>153</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>152</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>152</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="H2" s="17" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11"/>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="23"/>
-    </row>
-    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A4" s="15"/>
+      <c r="D3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+    </row>
+    <row r="4" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11"/>
       <c r="B4" s="3"/>
       <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="27"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="19"/>
-    </row>
-    <row r="5" spans="1:8" ht="15" customHeight="1">
-      <c r="A5" s="14" t="s">
+      <c r="D4" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="E4" s="23"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="15"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>25</v>
+        <v>158</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="29" t="s">
+      <c r="E5" s="25" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="11"/>
+      <c r="B6" s="13"/>
+      <c r="C6" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="G5" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" s="21" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="15" customHeight="1">
-      <c r="A6" s="15"/>
-      <c r="B6" s="17"/>
-      <c r="C6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32"/>
-      <c r="G6" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A7" s="15"/>
+      <c r="H6" s="19"/>
+    </row>
+    <row r="7" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="11"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="28"/>
-      <c r="G7" s="18" t="s">
+      <c r="E7" s="29"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="15"/>
+    </row>
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="H7" s="19"/>
-    </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1">
-      <c r="A8" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="F8" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="G8" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H8" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1">
-      <c r="A9" s="15"/>
+      <c r="G8" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H8" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="F9" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="22"/>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A10" s="15"/>
+        <v>74</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="19"/>
+    </row>
+    <row r="10" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="11"/>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
-      <c r="E10" s="33"/>
-      <c r="F10" s="28"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="19"/>
-    </row>
-    <row r="11" spans="1:8" ht="15" customHeight="1">
-      <c r="A11" s="14" t="s">
+      <c r="E10" s="29"/>
+      <c r="F10" s="24"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="15"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="1" t="s">
-        <v>50</v>
-      </c>
       <c r="D11" s="1"/>
-      <c r="E11" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="G11" s="20" t="s">
-        <v>77</v>
-      </c>
-      <c r="H11" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" ht="15" customHeight="1">
-      <c r="A12" s="15"/>
+      <c r="E11" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G11" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="11"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="31"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="H12" s="23"/>
-    </row>
-    <row r="13" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="16"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="12"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="28"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="19"/>
-    </row>
-    <row r="14" spans="1:8" ht="15" customHeight="1">
-      <c r="A14" s="14" t="s">
+      <c r="E13" s="29"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="15"/>
+    </row>
+    <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="29" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="30" t="s">
+      <c r="E14" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="16" t="s">
+        <v>49</v>
+      </c>
+      <c r="H14" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="G14" s="20" t="s">
+    </row>
+    <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="11"/>
+      <c r="B15" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="15" customHeight="1">
-      <c r="A15" s="15"/>
-      <c r="B15" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>57</v>
-      </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="31" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="32"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A16" s="16"/>
+      <c r="E15" s="27" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="28"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="28"/>
-      <c r="G16" s="18"/>
-      <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1">
-      <c r="A17" s="14" t="s">
+      <c r="E16" s="29"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="14"/>
+      <c r="H16" s="15"/>
+    </row>
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D17" s="1"/>
+      <c r="E17" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="F17" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C17" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="1"/>
-      <c r="E17" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="G17" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="H17" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1">
-      <c r="A18" s="15"/>
+      <c r="G17" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="11"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
-      <c r="E18" s="31" t="s">
-        <v>63</v>
-      </c>
-      <c r="F18" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G18" s="22"/>
-      <c r="H18" s="23"/>
-    </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="16"/>
+      <c r="E18" s="27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>57</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="12"/>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="28" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="18"/>
-      <c r="H19" s="19"/>
-    </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1">
-      <c r="A20" s="14" t="s">
+      <c r="E19" s="29"/>
+      <c r="F19" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="G19" s="14"/>
+      <c r="H19" s="15"/>
+    </row>
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10" t="s">
         <v>6</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="D20" s="1"/>
-      <c r="E20" s="29" t="s">
-        <v>127</v>
-      </c>
-      <c r="F20" s="30" t="s">
-        <v>127</v>
-      </c>
-      <c r="G20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H20" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1">
-      <c r="A21" s="15"/>
+      <c r="E20" s="25" t="s">
+        <v>117</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H20" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="11"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
-      <c r="E21" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="F21" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="G21" s="22"/>
-      <c r="H21" s="23"/>
-    </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A22" s="16"/>
+      <c r="E21" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>81</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19"/>
+    </row>
+    <row r="22" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="12"/>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="18"/>
-      <c r="H22" s="19"/>
-    </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1">
-      <c r="A23" s="14" t="s">
+      <c r="E22" s="29"/>
+      <c r="F22" s="24"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="15"/>
+    </row>
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="E23" s="29" t="s">
-        <v>81</v>
-      </c>
-      <c r="F23" s="30" t="s">
-        <v>81</v>
-      </c>
-      <c r="G23" s="20" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1">
-      <c r="A24" s="15"/>
+        <v>83</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F23" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="11"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="D24" s="2"/>
-      <c r="E24" s="31" t="s">
-        <v>82</v>
-      </c>
-      <c r="F24" s="32" t="s">
-        <v>84</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="H24" s="23" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A25" s="16"/>
+      <c r="E24" s="27" t="s">
+        <v>161</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>162</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>163</v>
+      </c>
+      <c r="H24" s="19" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="12"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="33" t="s">
-        <v>79</v>
-      </c>
-      <c r="F25" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="G25" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="H25" s="19"/>
-    </row>
-    <row r="26" spans="1:8" ht="15" customHeight="1">
-      <c r="A26" s="14" t="s">
+      <c r="E25" s="29" t="s">
+        <v>165</v>
+      </c>
+      <c r="F25" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="H25" s="15"/>
+    </row>
+    <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="10" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D26" s="1"/>
-      <c r="E26" s="34" t="s">
-        <v>72</v>
-      </c>
-      <c r="F26" s="30" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" s="24" t="s">
-        <v>45</v>
-      </c>
-      <c r="H26" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="15" customHeight="1">
-      <c r="A27" s="15"/>
+      <c r="E26" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="G26" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="H26" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="11"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="35" t="s">
-        <v>73</v>
-      </c>
-      <c r="F27" s="32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" s="25"/>
-      <c r="H27" s="23"/>
-    </row>
-    <row r="28" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A28" s="16"/>
+      <c r="E27" s="31" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>71</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="19"/>
+    </row>
+    <row r="28" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="12"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
-      <c r="E28" s="27" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="26"/>
-      <c r="H28" s="19"/>
-    </row>
-    <row r="29" spans="1:8" ht="15" customHeight="1">
-      <c r="A29" s="14" t="s">
+      <c r="E28" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="F28" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="22"/>
+      <c r="H28" s="15"/>
+    </row>
+    <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="D29" s="1"/>
-      <c r="E29" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F29" s="30" t="s">
-        <v>96</v>
-      </c>
-      <c r="G29" s="20" t="s">
-        <v>96</v>
-      </c>
-      <c r="H29" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="15" customHeight="1">
-      <c r="A30" s="15"/>
+      <c r="E29" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F29" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="11"/>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="31"/>
-      <c r="F30" s="32" t="s">
-        <v>97</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="H30" s="23"/>
-    </row>
-    <row r="31" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A31" s="16"/>
+      <c r="E30" s="27"/>
+      <c r="F30" s="28" t="s">
+        <v>87</v>
+      </c>
+      <c r="G30" s="18" t="s">
+        <v>88</v>
+      </c>
+      <c r="H30" s="19"/>
+    </row>
+    <row r="31" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
-      <c r="E31" s="33"/>
-      <c r="F31" s="28"/>
-      <c r="G31" s="18"/>
-      <c r="H31" s="19"/>
-    </row>
-    <row r="32" spans="1:8" ht="15" customHeight="1">
-      <c r="A32" s="14" t="s">
+      <c r="E31" s="29"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="15"/>
+    </row>
+    <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="10" t="s">
         <v>10</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D32" s="1"/>
-      <c r="E32" s="29" t="s">
-        <v>102</v>
-      </c>
-      <c r="F32" s="30" t="s">
-        <v>101</v>
-      </c>
-      <c r="G32" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H32" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="15" customHeight="1">
-      <c r="A33" s="15"/>
+      <c r="E32" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="F32" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="G32" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H32" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="31"/>
-      <c r="F33" s="32"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="23"/>
-    </row>
-    <row r="34" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A34" s="16"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="18"/>
+      <c r="H33" s="19"/>
+    </row>
+    <row r="34" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="12"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="28"/>
-      <c r="G34" s="18"/>
-      <c r="H34" s="19"/>
-    </row>
-    <row r="35" spans="1:8" ht="15" customHeight="1">
-      <c r="A35" s="14" t="s">
+      <c r="E34" s="29"/>
+      <c r="F34" s="24"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="15"/>
+    </row>
+    <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10" t="s">
         <v>11</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="D35" s="1"/>
-      <c r="E35" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="F35" s="30" t="s">
-        <v>105</v>
-      </c>
-      <c r="G35" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="H35" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" ht="15" customHeight="1">
-      <c r="A36" s="15"/>
+      <c r="E35" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>95</v>
+      </c>
+      <c r="G35" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="11"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
-      <c r="G36" s="22" t="s">
-        <v>106</v>
-      </c>
-      <c r="H36" s="23"/>
-    </row>
-    <row r="37" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A37" s="16"/>
+      <c r="E36" s="27"/>
+      <c r="F36" s="28"/>
+      <c r="G36" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="H36" s="19"/>
+    </row>
+    <row r="37" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="12"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
-      <c r="E37" s="33"/>
-      <c r="F37" s="28"/>
-      <c r="G37" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="H37" s="19"/>
-    </row>
-    <row r="38" spans="1:8" ht="15" customHeight="1">
-      <c r="A38" s="14" t="s">
+      <c r="E37" s="29"/>
+      <c r="F37" s="24"/>
+      <c r="G37" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="H37" s="15"/>
+    </row>
+    <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="D38" s="1"/>
-      <c r="E38" s="29" t="s">
-        <v>115</v>
-      </c>
-      <c r="F38" s="30" t="s">
-        <v>113</v>
-      </c>
-      <c r="G38" s="20" t="s">
-        <v>112</v>
-      </c>
-      <c r="H38" s="21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="15" customHeight="1">
-      <c r="A39" s="15"/>
+      <c r="E38" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38" s="26" t="s">
+        <v>103</v>
+      </c>
+      <c r="G38" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="H38" s="17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="11"/>
       <c r="B39" s="2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
-      <c r="E39" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="F39" s="32"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="23"/>
-    </row>
-    <row r="40" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A40" s="16"/>
+      <c r="E39" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39" s="28"/>
+      <c r="G39" s="18"/>
+      <c r="H39" s="19"/>
+    </row>
+    <row r="40" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="12"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
-      <c r="E40" s="33"/>
-      <c r="F40" s="28"/>
-      <c r="G40" s="18"/>
-      <c r="H40" s="19"/>
-    </row>
-    <row r="41" spans="1:8" ht="15" customHeight="1">
-      <c r="A41" s="14" t="s">
+      <c r="E40" s="29"/>
+      <c r="F40" s="24"/>
+      <c r="G40" s="14"/>
+      <c r="H40" s="15"/>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="10" t="s">
         <v>13</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="E41" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>166</v>
+      </c>
+      <c r="F41" s="26" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="11"/>
+      <c r="B42" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E42" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="F42" s="28" t="s">
+        <v>109</v>
+      </c>
+      <c r="G42" s="18"/>
+      <c r="H42" s="19"/>
+    </row>
+    <row r="43" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="12"/>
+      <c r="B43" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E43" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="F43" s="24"/>
+      <c r="G43" s="14"/>
+      <c r="H43" s="15"/>
+    </row>
+    <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B44" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="F41" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="G41" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H41" s="21" t="s">
+      <c r="C44" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="25" t="s">
+        <v>121</v>
+      </c>
+      <c r="F44" s="26"/>
+      <c r="G44" s="16"/>
+      <c r="H44" s="17" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="15" customHeight="1">
-      <c r="A42" s="15"/>
-      <c r="B42" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="E42" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="F42" s="32" t="s">
-        <v>119</v>
-      </c>
-      <c r="G42" s="22"/>
-      <c r="H42" s="23"/>
-    </row>
-    <row r="43" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="E43" s="33"/>
-      <c r="F43" s="28"/>
-      <c r="G43" s="18"/>
-      <c r="H43" s="19"/>
-    </row>
-    <row r="44" spans="1:8" ht="15" customHeight="1">
-      <c r="A44" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D44" s="1"/>
-      <c r="E44" s="29" t="s">
-        <v>131</v>
-      </c>
-      <c r="F44" s="30"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="21" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" ht="15" customHeight="1">
-      <c r="A45" s="15"/>
+    <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="11"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="32"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="23"/>
-    </row>
-    <row r="46" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A46" s="16"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="28"/>
+      <c r="G45" s="18"/>
+      <c r="H45" s="19"/>
+    </row>
+    <row r="46" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="12"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
-      <c r="E46" s="33"/>
-      <c r="F46" s="28"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="19"/>
-    </row>
-    <row r="47" spans="1:8" ht="15" customHeight="1">
-      <c r="A47" s="14" t="s">
+      <c r="E46" s="29"/>
+      <c r="F46" s="24"/>
+      <c r="G46" s="14"/>
+      <c r="H46" s="15"/>
+    </row>
+    <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>15</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="D47" s="1"/>
-      <c r="E47" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F47" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="G47" s="20" t="s">
-        <v>136</v>
-      </c>
-      <c r="H47" s="21" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" ht="15" customHeight="1">
-      <c r="A48" s="15"/>
+      <c r="E47" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G47" s="16" t="s">
+        <v>126</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="11"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="23"/>
-    </row>
-    <row r="49" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A49" s="16"/>
+      <c r="E48" s="27"/>
+      <c r="F48" s="28"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="19"/>
+    </row>
+    <row r="49" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="12"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
-      <c r="E49" s="33"/>
-      <c r="F49" s="28"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="19"/>
-    </row>
-    <row r="50" spans="1:8" ht="15" customHeight="1">
-      <c r="A50" s="14" t="s">
+      <c r="E49" s="29"/>
+      <c r="F49" s="24"/>
+      <c r="G49" s="14"/>
+      <c r="H49" s="15"/>
+    </row>
+    <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="10" t="s">
         <v>16</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="D50" s="1"/>
-      <c r="E50" s="29" t="s">
-        <v>45</v>
-      </c>
-      <c r="F50" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="G50" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="H50" s="21" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" ht="15" customHeight="1">
-      <c r="A51" s="15"/>
+      <c r="E50" s="25" t="s">
+        <v>41</v>
+      </c>
+      <c r="F50" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="G50" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="H50" s="17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="11"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="23"/>
-    </row>
-    <row r="52" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A52" s="16"/>
+      <c r="E51" s="27"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="19"/>
+    </row>
+    <row r="52" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="12"/>
       <c r="B52" s="3"/>
       <c r="C52" s="3"/>
       <c r="D52" s="3"/>
-      <c r="E52" s="33"/>
-      <c r="F52" s="28"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="19"/>
-    </row>
-    <row r="53" spans="1:8" ht="15" customHeight="1">
-      <c r="A53" s="14" t="s">
+      <c r="E52" s="29"/>
+      <c r="F52" s="24"/>
+      <c r="G52" s="14"/>
+      <c r="H52" s="15"/>
+    </row>
+    <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="10" t="s">
         <v>17</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="D53" s="1"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="30" t="s">
-        <v>138</v>
-      </c>
-      <c r="G53" s="20"/>
-      <c r="H53" s="21" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" ht="15" customHeight="1">
-      <c r="A54" s="15"/>
+      <c r="E53" s="25"/>
+      <c r="F53" s="26" t="s">
+        <v>128</v>
+      </c>
+      <c r="G53" s="16"/>
+      <c r="H53" s="17" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="11"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2" t="s">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="D54" s="2"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32" t="s">
-        <v>143</v>
-      </c>
-      <c r="G54" s="22"/>
-      <c r="H54" s="23" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A55" s="16"/>
+      <c r="E54" s="27"/>
+      <c r="F54" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="G54" s="18"/>
+      <c r="H54" s="19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="12"/>
       <c r="B55" s="3"/>
       <c r="C55" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="29"/>
+      <c r="F55" s="24"/>
+      <c r="G55" s="14"/>
+      <c r="H55" s="15"/>
+    </row>
+    <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="25" t="s">
+        <v>136</v>
+      </c>
+      <c r="F56" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="G56" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="D55" s="3"/>
-      <c r="E55" s="33"/>
-      <c r="F55" s="28"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="19"/>
-    </row>
-    <row r="56" spans="1:8" ht="15" customHeight="1">
-      <c r="A56" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="C56" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D56" s="1"/>
-      <c r="E56" s="29" t="s">
-        <v>146</v>
-      </c>
-      <c r="F56" s="30" t="s">
-        <v>148</v>
-      </c>
-      <c r="G56" s="20" t="s">
-        <v>150</v>
-      </c>
-      <c r="H56" s="21" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" ht="15" customHeight="1">
-      <c r="A57" s="15"/>
+      <c r="H56" s="17" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="11"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="F57" s="32" t="s">
-        <v>153</v>
-      </c>
-      <c r="G57" s="22" t="s">
-        <v>149</v>
-      </c>
-      <c r="H57" s="23" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A58" s="16"/>
+      <c r="E57" s="27" t="s">
+        <v>137</v>
+      </c>
+      <c r="F57" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="H57" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A58" s="12"/>
       <c r="B58" s="3"/>
       <c r="C58" s="3"/>
       <c r="D58" s="3"/>
-      <c r="E58" s="33"/>
-      <c r="F58" s="28"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="19"/>
-    </row>
-    <row r="59" spans="1:8" ht="15" customHeight="1">
-      <c r="A59" s="14" t="s">
+      <c r="E58" s="29"/>
+      <c r="F58" s="24"/>
+      <c r="G58" s="14"/>
+      <c r="H58" s="15"/>
+    </row>
+    <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="10" t="s">
         <v>19</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D59" s="1"/>
-      <c r="E59" s="29" t="s">
-        <v>158</v>
-      </c>
-      <c r="F59" s="30" t="s">
-        <v>159</v>
-      </c>
-      <c r="G59" s="20"/>
-      <c r="H59" s="21" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" ht="15" customHeight="1">
-      <c r="A60" s="15"/>
+      <c r="E59" s="25" t="s">
+        <v>148</v>
+      </c>
+      <c r="F59" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="G59" s="16"/>
+      <c r="H59" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
       <c r="B60" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
-      <c r="E60" s="31"/>
-      <c r="F60" s="32"/>
-      <c r="G60" s="22"/>
-      <c r="H60" s="23"/>
-    </row>
-    <row r="61" spans="1:8" ht="15" customHeight="1" thickBot="1">
-      <c r="A61" s="16"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="28"/>
+      <c r="G60" s="18"/>
+      <c r="H60" s="19"/>
+    </row>
+    <row r="61" spans="1:8" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="12"/>
       <c r="B61" s="3" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C61" s="3"/>
       <c r="D61" s="3"/>
-      <c r="E61" s="33"/>
-      <c r="F61" s="28"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="19"/>
-    </row>
-    <row r="62" spans="1:8" ht="15" customHeight="1">
-      <c r="A62" s="7"/>
-      <c r="B62" s="7"/>
-      <c r="C62" s="7"/>
-      <c r="D62" s="7"/>
-      <c r="E62" s="7"/>
-      <c r="F62" s="7"/>
-      <c r="G62" s="7"/>
-      <c r="H62" s="7"/>
+      <c r="E61" s="29"/>
+      <c r="F61" s="24"/>
+      <c r="G61" s="14"/>
+      <c r="H61" s="15"/>
+    </row>
+    <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="5"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>